<commit_message>
added seir simulatons for all pathogens
</commit_message>
<xml_diff>
--- a/par-calculator.xlsx
+++ b/par-calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/code/operation-outbreak/oo-models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/code/operation-outbreak/oo-parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE8F721-A969-D943-AFB4-EF4EE162E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0B1B1B-A813-D649-AC93-40D8E47F041B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="22160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EPI Calculation Formulas" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -485,7 +485,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -727,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:AA1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -744,10 +743,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
+      <c r="C1" s="21"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
         <v>100</v>
@@ -777,8 +776,8 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="3"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -808,11 +807,11 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="21">
-        <v>5</v>
+      <c r="C3" s="3">
+        <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
@@ -847,10 +846,10 @@
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4">
         <v>0.5</v>
       </c>
       <c r="D4" s="3"/>
@@ -890,11 +889,11 @@
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21">
-        <v>0.2</v>
+      <c r="C5" s="3">
+        <v>0.1</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5"/>
@@ -925,11 +924,11 @@
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="20">
-        <v>0.02</v>
+      <c r="C6">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
@@ -964,11 +963,11 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="21">
-        <v>0.3</v>
+      <c r="C7" s="3">
+        <v>2</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="5"/>
@@ -999,11 +998,11 @@
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="21">
-        <v>2.4</v>
+      <c r="C8" s="3">
+        <v>3</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="5" t="s">
@@ -1036,11 +1035,11 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="21">
-        <v>0.5</v>
+      <c r="C9" s="3">
+        <v>1</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="6" t="s">
@@ -1075,10 +1074,10 @@
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3"/>
@@ -1116,10 +1115,10 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="3"/>
@@ -1149,10 +1148,10 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="29" t="s">
         <v>71</v>
       </c>
       <c r="F12" s="5">
@@ -1186,10 +1185,10 @@
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="3">
         <v>0.3</v>
       </c>
       <c r="D13" s="3"/>
@@ -1221,11 +1220,11 @@
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="21">
-        <v>0.7</v>
+      <c r="C14" s="3">
+        <v>0.6</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="6" t="s">
@@ -1261,14 +1260,14 @@
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="21">
-        <v>0.5</v>
+      <c r="C15" s="3">
+        <v>0.4</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="F15" s="27"/>
+      <c r="F15" s="26"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1294,11 +1293,11 @@
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="21">
-        <v>0.86</v>
+      <c r="C16" s="3">
+        <v>0.6</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="7" t="s">
@@ -1331,11 +1330,11 @@
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="21">
-        <v>0.7</v>
+      <c r="C17" s="3">
+        <v>0.1</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="7"/>
@@ -1364,12 +1363,12 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <f>C5+C14+(1-C14+C14*C15)*C7</f>
-        <v>1.095</v>
+        <v>1.98</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="7"/>
@@ -1398,12 +1397,12 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="20">
         <f>C22*(C13*(C8-C18)+C18)</f>
-        <v>0.74830103196576903</v>
+        <v>0.8205312275664034</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="7" t="s">
@@ -1505,7 +1504,7 @@
       </c>
       <c r="C22" s="10">
         <f>F3/(F6*(C4+C13*(C8-C18)+C18))</f>
-        <v>0.50339793606846217</v>
+        <v>0.35893754486719309</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="7"/>
@@ -1541,7 +1540,7 @@
       </c>
       <c r="C23" s="10">
         <f>(C3*F10)/(F12*F9*C19*F14)</f>
-        <v>7.4242254363344161E-4</v>
+        <v>9.4789540196364339E-4</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="7"/>
@@ -1575,7 +1574,7 @@
       </c>
       <c r="C24" s="10">
         <f>C9*C23</f>
-        <v>3.712112718167208E-4</v>
+        <v>9.4789540196364339E-4</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="7"/>
@@ -1609,7 +1608,7 @@
       </c>
       <c r="C25" s="10">
         <f>C10*C23</f>
-        <v>7.4242254363344161E-4</v>
+        <v>9.4789540196364339E-4</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="7"/>
@@ -1643,7 +1642,7 @@
       </c>
       <c r="C26" s="10">
         <f>C11*C23</f>
-        <v>7.4242254363344161E-4</v>
+        <v>9.4789540196364339E-4</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="7"/>
@@ -1677,7 +1676,7 @@
       </c>
       <c r="C27" s="10">
         <f>C4*C22</f>
-        <v>0.25169896803423109</v>
+        <v>0.17946877243359655</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="7"/>
@@ -1711,7 +1710,7 @@
       </c>
       <c r="C28" s="10">
         <f>C7*C22</f>
-        <v>0.15101938082053865</v>
+        <v>0.71787508973438618</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1745,7 +1744,7 @@
       </c>
       <c r="C29" s="10">
         <f>$C5*$C22</f>
-        <v>0.10067958721369244</v>
+        <v>3.5893754486719311E-2</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="11" t="s">
@@ -1781,7 +1780,7 @@
       </c>
       <c r="C30" s="10">
         <f>C6*C22</f>
-        <v>1.0067958721369244E-2</v>
+        <v>5.3840631730078959E-3</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="12" t="s">
@@ -1819,7 +1818,7 @@
       </c>
       <c r="C31" s="10">
         <f>$C8*$C22</f>
-        <v>1.2081550465643092</v>
+        <v>1.0768126346015792</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="12" t="s">
@@ -2049,7 +2048,7 @@
       </c>
       <c r="C38" s="15">
         <f>C3/C19</f>
-        <v>6.6818028927009747</v>
+        <v>8.5310586176727909</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -2083,7 +2082,7 @@
       </c>
       <c r="C39" s="13">
         <f>1/C19</f>
-        <v>1.3363605785401949</v>
+        <v>1.2187226596675416</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -2117,7 +2116,7 @@
       </c>
       <c r="C40" s="13">
         <f>1/$C27</f>
-        <v>3.9729999999999994</v>
+        <v>5.5720000000000001</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -30410,10 +30409,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -30541,7 +30540,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>23</v>
       </c>
     </row>
@@ -30599,7 +30598,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>61</v>
       </c>
     </row>
@@ -30615,7 +30614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1131AB-CE15-5A4C-ABE2-DA91D162E67B}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -30624,10 +30625,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -30755,7 +30756,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>23</v>
       </c>
     </row>
@@ -30811,7 +30812,7 @@
       <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29"/>
+      <c r="A28" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30822,7 +30823,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B132E5-5A8B-7C4F-887F-BF1E9B9551E4}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -30831,10 +30834,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -30962,7 +30965,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>55</v>
       </c>
     </row>
@@ -31020,17 +31023,17 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>67</v>
       </c>
     </row>
@@ -31047,7 +31050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8F25E9-80DD-4F46-A150-0D1211E7E472}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView topLeftCell="B2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -31056,10 +31061,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -31187,7 +31192,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>81</v>
       </c>
     </row>
@@ -31245,17 +31250,17 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>67</v>
       </c>
     </row>
@@ -31272,7 +31277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D68CC4B-0DA8-C14A-B8A7-F18D100FE9A5}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -31281,10 +31288,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -31412,7 +31419,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>55</v>
       </c>
     </row>
@@ -31470,15 +31477,15 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="29"/>
+      <c r="A29" s="28"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="29"/>
+      <c r="A30" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31489,7 +31496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FD915A-0A31-FD43-A30E-ED6BE6895338}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -31498,10 +31507,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -31629,7 +31638,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>81</v>
       </c>
     </row>
@@ -31685,13 +31694,13 @@
       <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29"/>
+      <c r="A28" s="28"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="29"/>
+      <c r="A29" s="28"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="29"/>
+      <c r="A30" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31702,7 +31711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4966E832-9944-D544-886B-D77EBEEF54A6}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -31711,10 +31722,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -31842,7 +31853,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>55</v>
       </c>
     </row>
@@ -31900,17 +31911,17 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>97</v>
       </c>
     </row>
@@ -31923,7 +31934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EC3D12-1968-714F-854F-7AA72F889577}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -31932,10 +31945,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -32063,7 +32076,7 @@
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>23</v>
       </c>
     </row>
@@ -32119,13 +32132,13 @@
       <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="29"/>
+      <c r="A28" s="28"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="29"/>
+      <c r="A29" s="28"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="29"/>
+      <c r="A30" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added parameter to account for fraction of population using the app
</commit_message>
<xml_diff>
--- a/par-calculator.xlsx
+++ b/par-calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/code/operation-outbreak/oo-parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0B1B1B-A813-D649-AC93-40D8E47F041B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380A5334-568F-5A49-8BA9-4F50FCD4C2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EPI Calculation Formulas" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="103">
   <si>
     <t>Simulation-independent parameters</t>
   </si>
@@ -338,10 +338,16 @@
     <t>Simulation-independent parameters for novel virus X</t>
   </si>
   <si>
-    <t>conversion_constant (sim-time-unit-to-sim-step)</t>
+    <t>Simulation constrains and social mixing parameters</t>
   </si>
   <si>
-    <t>Simulation constrains and social mixing parameters</t>
+    <t>Conversion_constant (sim-time-unit-to-sim-step)</t>
+  </si>
+  <si>
+    <t>Percentage of population using the OO app</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -456,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -505,6 +511,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -726,8 +733,8 @@
   </sheetPr>
   <dimension ref="A1:AA1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C17"/>
+    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -749,7 +756,7 @@
       <c r="C1" s="21"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -810,7 +817,7 @@
       <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="20">
         <v>7</v>
       </c>
       <c r="D3" s="3"/>
@@ -849,7 +856,7 @@
       <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="30">
         <v>0.5</v>
       </c>
       <c r="D4" s="3"/>
@@ -892,7 +899,7 @@
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="20">
         <v>0.1</v>
       </c>
       <c r="D5" s="3"/>
@@ -927,7 +934,7 @@
       <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="30">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D6" s="3"/>
@@ -966,7 +973,7 @@
       <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="20">
         <v>2</v>
       </c>
       <c r="D7" s="3"/>
@@ -1001,7 +1008,7 @@
       <c r="B8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="3"/>
@@ -1038,7 +1045,7 @@
       <c r="B9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="20">
         <v>1</v>
       </c>
       <c r="D9" s="3"/>
@@ -1077,7 +1084,7 @@
       <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="20">
         <v>1</v>
       </c>
       <c r="D10" s="3"/>
@@ -1118,7 +1125,7 @@
       <c r="B11" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="20">
         <v>1</v>
       </c>
       <c r="D11" s="3"/>
@@ -1188,13 +1195,19 @@
       <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="20">
         <v>0.3</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="5">
+        <v>100</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1223,12 +1236,12 @@
       <c r="B14" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="20">
         <v>0.6</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="6" t="s">
-        <v>99</v>
+      <c r="E14" s="29" t="s">
+        <v>100</v>
       </c>
       <c r="F14" s="5">
         <f>G4*60/F19</f>
@@ -1263,7 +1276,7 @@
       <c r="B15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="20">
         <v>0.4</v>
       </c>
       <c r="D15" s="3"/>
@@ -1296,7 +1309,7 @@
       <c r="B16" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="20">
         <v>0.6</v>
       </c>
       <c r="D16" s="3"/>
@@ -1333,7 +1346,7 @@
       <c r="B17" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="20">
         <v>0.1</v>
       </c>
       <c r="D17" s="3"/>
@@ -1539,7 +1552,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="10">
-        <f>(C3*F10)/(F12*F9*C19*F14)</f>
+        <f>(C3*(F10*100/F13))/(F12*F9*C19*F14)</f>
         <v>9.4789540196364339E-4</v>
       </c>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
use the scaled R0 as aux var
</commit_message>
<xml_diff>
--- a/par-calculator.xlsx
+++ b/par-calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/code/operation-outbreak/oo-parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380A5334-568F-5A49-8BA9-4F50FCD4C2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341696F3-FECE-AB41-97B4-B0B42C5CA0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40960" yWindow="500" windowWidth="40940" windowHeight="22540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EPI Calculation Formulas" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="104">
   <si>
     <t>Simulation-independent parameters</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>inf_severe_to_inf_mild_ratio</t>
-  </si>
-  <si>
-    <t>Number of epi generations</t>
   </si>
   <si>
     <t>asym_to_inf_mild_ratio</t>
@@ -341,13 +338,19 @@
     <t>Simulation constrains and social mixing parameters</t>
   </si>
   <si>
-    <t>Conversion_constant (sim-time-unit-to-sim-step)</t>
+    <t>%</t>
   </si>
   <si>
-    <t>Percentage of population using the OO app</t>
+    <t>HELPER VALUE R0 scaled (do not overwrite)</t>
   </si>
   <si>
-    <t>%</t>
+    <t>Number of consecutive infections during simulation</t>
+  </si>
+  <si>
+    <t>Conversion constant (sim-time-unit-to-sim-step)</t>
+  </si>
+  <si>
+    <t>Percentage of target population using the OO app</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -512,6 +515,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -731,10 +735,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1015"/>
+  <dimension ref="A1:AA1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -756,7 +760,7 @@
       <c r="C1" s="21"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -812,17 +816,17 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="20">
         <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="5">
         <v>2</v>
@@ -851,7 +855,7 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>1</v>
@@ -861,16 +865,16 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="6">
         <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -894,7 +898,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>2</v>
@@ -929,7 +933,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>3</v>
@@ -939,7 +943,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
@@ -968,7 +972,7 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>4</v>
@@ -1003,17 +1007,17 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1040,17 +1044,17 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="20">
         <v>1</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5">
         <v>5</v>
@@ -1079,23 +1083,23 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="20">
         <v>1</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="5">
         <v>1</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="3"/>
@@ -1120,10 +1124,10 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="20">
         <v>1</v>
@@ -1159,13 +1163,13 @@
       <c r="C12" s="20"/>
       <c r="D12" s="3"/>
       <c r="E12" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
@@ -1190,23 +1194,23 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="20">
         <v>0.3</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="29" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F13" s="5">
         <v>100</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="3"/>
@@ -1231,17 +1235,17 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>15</v>
       </c>
       <c r="C14" s="20">
         <v>0.6</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="29" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F14" s="5">
         <f>G4*60/F19</f>
@@ -1271,10 +1275,10 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="20">
         <v>0.4</v>
@@ -1304,17 +1308,17 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="20">
         <v>0.6</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1341,10 +1345,10 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="20">
         <v>0.1</v>
@@ -1377,7 +1381,7 @@
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="20">
         <f>C5+C14+(1-C14+C14*C15)*C7</f>
@@ -1411,21 +1415,21 @@
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="20">
-        <f>C22*(C13*(C8-C18)+C18)</f>
+        <f>C23*(C13*(C8-C18)+C18)</f>
         <v>0.8205312275664034</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="7">
         <v>2</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="3"/>
@@ -1449,9 +1453,14 @@
       <c r="AA19" s="3"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="20">
+        <f>C3*(100/F13)</f>
+        <v>7</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1478,11 +1487,9 @@
       <c r="AA20" s="3"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="10"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1509,16 +1516,11 @@
       <c r="AA21" s="3"/>
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="10">
-        <f>F3/(F6*(C4+C13*(C8-C18)+C18))</f>
-        <v>0.35893754486719309</v>
-      </c>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="10"/>
       <c r="D22" s="3"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1546,14 +1548,14 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C23" s="10">
-        <f>(C3*(F10*100/F13))/(F12*F9*C19*F14)</f>
-        <v>9.4789540196364339E-4</v>
+        <f>F3/(F6*(C4+C13*(C8-C18)+C18))</f>
+        <v>0.35893754486719309</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="7"/>
@@ -1581,12 +1583,14 @@
       <c r="AA23" s="3"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="10"/>
+      <c r="A24" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="B24" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="10">
-        <f>C9*C23</f>
+        <f>(C20*F10)/(F12*F9*C19*F14)</f>
         <v>9.4789540196364339E-4</v>
       </c>
       <c r="D24" s="3"/>
@@ -1617,10 +1621,10 @@
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="10">
-        <f>C10*C23</f>
+        <f>C9*C24</f>
         <v>9.4789540196364339E-4</v>
       </c>
       <c r="D25" s="3"/>
@@ -1651,10 +1655,10 @@
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="10">
-        <f>C11*C23</f>
+        <f>C10*C24</f>
         <v>9.4789540196364339E-4</v>
       </c>
       <c r="D26" s="3"/>
@@ -1685,11 +1689,11 @@
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C27" s="10">
-        <f>C4*C22</f>
-        <v>0.17946877243359655</v>
+        <f>C11*C24</f>
+        <v>9.4789540196364339E-4</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="7"/>
@@ -1719,17 +1723,17 @@
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C28" s="10">
-        <f>C7*C22</f>
-        <v>0.71787508973438618</v>
+        <f>C4*C23</f>
+        <v>0.17946877243359655</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1753,19 +1757,17 @@
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C29" s="10">
-        <f>$C5*$C22</f>
-        <v>3.5893754486719311E-2</v>
+        <f>C7*C23</f>
+        <v>0.71787508973438618</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1789,19 +1791,17 @@
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C30" s="10">
-        <f>C6*C22</f>
-        <v>5.3840631730078959E-3</v>
+        <f>$C5*$C23</f>
+        <v>3.5893754486719311E-2</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="12">
-        <v>0.3</v>
-      </c>
+      <c r="E30" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
       <c r="I30" s="3"/>
@@ -1827,19 +1827,18 @@
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C31" s="10">
-        <f>$C8*$C22</f>
-        <v>1.0768126346015792</v>
+        <f>C6*C23</f>
+        <v>5.3840631730078959E-3</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F31" s="12">
-        <f>$F30/($F3*$F14*60/$F19)</f>
-        <v>2.7777777777777775E-6</v>
+        <v>0.3</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -1866,18 +1865,19 @@
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="10" t="str">
-        <f>$F4</f>
-        <v>hour</v>
+        <v>42</v>
+      </c>
+      <c r="C32" s="10">
+        <f>$C8*$C23</f>
+        <v>1.0768126346015792</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F32" s="12">
-        <v>2</v>
+        <f>$F31/($F3*$F14*60/$F19)</f>
+        <v>2.7777777777777775E-6</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
@@ -1902,9 +1902,17 @@
       <c r="AA32" s="3"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="10" t="str">
+        <f>$F4</f>
+        <v>hour</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F33" s="12">
         <v>2</v>
@@ -1932,15 +1940,12 @@
       <c r="AA33" s="3"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F34" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
@@ -1966,14 +1971,14 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>28</v>
+        <v>41</v>
+      </c>
+      <c r="F35" s="12">
+        <v>1</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -1998,11 +2003,18 @@
       <c r="AA35" s="3"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="E36" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2024,11 +2036,6 @@
       <c r="AA36" s="3"/>
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="13"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -2056,13 +2063,10 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13"/>
-      <c r="B38" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="15">
-        <f>C3/C19</f>
-        <v>8.5310586176727909</v>
-      </c>
+      <c r="B38" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="13"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -2091,11 +2095,11 @@
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="13"/>
       <c r="B39" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="13">
-        <f>1/C19</f>
-        <v>1.2187226596675416</v>
+        <v>49</v>
+      </c>
+      <c r="C39" s="15">
+        <f>C3/C19</f>
+        <v>8.5310586176727909</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -2125,11 +2129,11 @@
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="13"/>
       <c r="B40" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" s="13">
-        <f>1/$C27</f>
-        <v>5.5720000000000001</v>
+        <f>1/C19</f>
+        <v>1.2187226596675416</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -2157,6 +2161,14 @@
       <c r="AA40" s="3"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="13">
+        <f>1/$C28</f>
+        <v>5.5720000000000001</v>
+      </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -2209,9 +2221,6 @@
       <c r="AA42" s="3"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -2817,7 +2826,7 @@
       <c r="Z63" s="3"/>
       <c r="AA63" s="3"/>
     </row>
-    <row r="64" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -30222,7 +30231,10 @@
       <c r="Z1008" s="3"/>
       <c r="AA1008" s="3"/>
     </row>
-    <row r="1009" spans="4:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="1009" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1009" s="3"/>
+      <c r="B1009" s="3"/>
+      <c r="C1009" s="3"/>
       <c r="D1009" s="3"/>
       <c r="E1009" s="3"/>
       <c r="F1009" s="3"/>
@@ -30248,7 +30260,7 @@
       <c r="Z1009" s="3"/>
       <c r="AA1009" s="3"/>
     </row>
-    <row r="1010" spans="4:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="1010" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="D1010" s="3"/>
       <c r="E1010" s="3"/>
       <c r="F1010" s="3"/>
@@ -30274,7 +30286,7 @@
       <c r="Z1010" s="3"/>
       <c r="AA1010" s="3"/>
     </row>
-    <row r="1011" spans="4:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="1011" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="D1011" s="3"/>
       <c r="E1011" s="3"/>
       <c r="F1011" s="3"/>
@@ -30300,7 +30312,7 @@
       <c r="Z1011" s="3"/>
       <c r="AA1011" s="3"/>
     </row>
-    <row r="1012" spans="4:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="1012" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="D1012" s="3"/>
       <c r="E1012" s="3"/>
       <c r="F1012" s="3"/>
@@ -30326,7 +30338,7 @@
       <c r="Z1012" s="3"/>
       <c r="AA1012" s="3"/>
     </row>
-    <row r="1013" spans="4:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="1013" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="D1013" s="3"/>
       <c r="E1013" s="3"/>
       <c r="F1013" s="3"/>
@@ -30352,7 +30364,7 @@
       <c r="Z1013" s="3"/>
       <c r="AA1013" s="3"/>
     </row>
-    <row r="1014" spans="4:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="1014" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="D1014" s="3"/>
       <c r="E1014" s="3"/>
       <c r="F1014" s="3"/>
@@ -30378,7 +30390,7 @@
       <c r="Z1014" s="3"/>
       <c r="AA1014" s="3"/>
     </row>
-    <row r="1015" spans="4:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="1015" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="D1015" s="3"/>
       <c r="E1015" s="3"/>
       <c r="F1015" s="3"/>
@@ -30404,6 +30416,32 @@
       <c r="Z1015" s="3"/>
       <c r="AA1015" s="3"/>
     </row>
+    <row r="1016" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+      <c r="D1016" s="3"/>
+      <c r="E1016" s="3"/>
+      <c r="F1016" s="3"/>
+      <c r="G1016" s="3"/>
+      <c r="H1016" s="3"/>
+      <c r="I1016" s="3"/>
+      <c r="J1016" s="3"/>
+      <c r="K1016" s="3"/>
+      <c r="L1016" s="3"/>
+      <c r="M1016" s="3"/>
+      <c r="N1016" s="3"/>
+      <c r="O1016" s="3"/>
+      <c r="P1016" s="3"/>
+      <c r="Q1016" s="3"/>
+      <c r="R1016" s="3"/>
+      <c r="S1016" s="3"/>
+      <c r="T1016" s="3"/>
+      <c r="U1016" s="3"/>
+      <c r="V1016" s="3"/>
+      <c r="W1016" s="3"/>
+      <c r="X1016" s="3"/>
+      <c r="Y1016" s="3"/>
+      <c r="Z1016" s="3"/>
+      <c r="AA1016" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30423,7 +30461,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -30435,7 +30473,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -30475,7 +30513,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>2.4</v>
@@ -30483,7 +30521,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>0.5</v>
@@ -30491,7 +30529,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -30499,7 +30537,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -30511,7 +30549,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0.3</v>
@@ -30519,7 +30557,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0.7</v>
@@ -30527,7 +30565,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0.5</v>
@@ -30535,7 +30573,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0.86</v>
@@ -30543,7 +30581,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.7</v>
@@ -30551,15 +30589,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>22</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -30567,7 +30605,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -30575,7 +30613,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
@@ -30583,15 +30621,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
@@ -30599,20 +30637,20 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -30639,7 +30677,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -30651,7 +30689,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -30691,7 +30729,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>0.83</v>
@@ -30699,7 +30737,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>0.8</v>
@@ -30707,7 +30745,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -30715,7 +30753,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1.5</v>
@@ -30727,7 +30765,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0.4</v>
@@ -30735,7 +30773,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0.65</v>
@@ -30743,7 +30781,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0.3</v>
@@ -30751,7 +30789,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0.95</v>
@@ -30759,7 +30797,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.83</v>
@@ -30767,15 +30805,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>22</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -30783,7 +30821,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -30791,7 +30829,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -30799,15 +30837,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -30815,10 +30853,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
@@ -30848,7 +30886,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -30860,7 +30898,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -30900,7 +30938,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>0.5</v>
@@ -30908,7 +30946,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>0.9</v>
@@ -30916,7 +30954,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -30924,7 +30962,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -30936,7 +30974,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0.1</v>
@@ -30944,7 +30982,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0.3</v>
@@ -30952,7 +30990,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0.7</v>
@@ -30960,7 +30998,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0.8</v>
@@ -30968,7 +31006,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.4</v>
@@ -30976,15 +31014,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -30992,7 +31030,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -31000,7 +31038,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -31008,15 +31046,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -31024,30 +31062,30 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -31075,7 +31113,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31087,7 +31125,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>17</v>
@@ -31127,7 +31165,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -31135,7 +31173,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -31143,7 +31181,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -31151,7 +31189,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -31163,7 +31201,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -31171,7 +31209,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -31179,7 +31217,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -31187,7 +31225,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -31195,7 +31233,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.98</v>
@@ -31203,15 +31241,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -31219,7 +31257,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -31227,7 +31265,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
@@ -31235,15 +31273,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
@@ -31251,30 +31289,30 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -31302,7 +31340,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31314,7 +31352,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -31354,7 +31392,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>2.5</v>
@@ -31362,7 +31400,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>0.5</v>
@@ -31370,7 +31408,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -31378,7 +31416,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -31390,7 +31428,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0.5</v>
@@ -31398,7 +31436,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -31406,7 +31444,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -31414,7 +31452,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -31422,7 +31460,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -31430,15 +31468,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -31446,7 +31484,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -31454,7 +31492,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -31462,15 +31500,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -31478,20 +31516,20 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
@@ -31521,7 +31559,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31533,7 +31571,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -31573,7 +31611,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>0.5</v>
@@ -31581,7 +31619,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -31589,7 +31627,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -31597,7 +31635,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -31609,7 +31647,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0.2</v>
@@ -31617,7 +31655,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0.8</v>
@@ -31625,7 +31663,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0.1</v>
@@ -31633,7 +31671,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0.95</v>
@@ -31641,7 +31679,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.84</v>
@@ -31649,15 +31687,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -31665,7 +31703,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -31673,7 +31711,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
@@ -31681,15 +31719,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -31697,10 +31735,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
@@ -31736,7 +31774,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31748,7 +31786,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -31788,7 +31826,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -31796,7 +31834,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>0.5</v>
@@ -31804,7 +31842,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -31812,7 +31850,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -31824,7 +31862,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0.3</v>
@@ -31832,7 +31870,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0.5</v>
@@ -31840,7 +31878,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0.3</v>
@@ -31848,7 +31886,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0.91</v>
@@ -31856,7 +31894,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.71</v>
@@ -31864,15 +31902,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -31880,7 +31918,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -31888,7 +31926,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
@@ -31896,15 +31934,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -31912,30 +31950,30 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -31959,7 +31997,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31971,7 +32009,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>7</v>
@@ -32011,7 +32049,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -32019,7 +32057,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -32027,7 +32065,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -32035,7 +32073,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -32047,7 +32085,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>0.3</v>
@@ -32055,7 +32093,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0.6</v>
@@ -32063,7 +32101,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0.4</v>
@@ -32071,7 +32109,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>0.6</v>
@@ -32079,7 +32117,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>0.1</v>
@@ -32087,15 +32125,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>22</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -32103,7 +32141,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -32111,7 +32149,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -32119,15 +32157,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -32135,10 +32173,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
added detection rate to parameter calculator
</commit_message>
<xml_diff>
--- a/par-calculator.xlsx
+++ b/par-calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/code/operation-outbreak/oo-parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1562462-91ED-F14B-8E82-DF4B5F778896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9FBF23-E0CE-7C45-A415-8EB30BDB45A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="40940" windowHeight="22540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="105">
   <si>
     <t>Simulation-independent parameters</t>
   </si>
@@ -254,9 +254,6 @@
     <t>Mean contact duration</t>
   </si>
   <si>
-    <t>seconds</t>
-  </si>
-  <si>
     <t>Total duration of simulation</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
   </si>
   <si>
     <t>hour</t>
-  </si>
-  <si>
-    <t>Time unit of simulation (if change, UPDATE G4 value)</t>
   </si>
   <si>
     <t>Simulation-independent parameters for Measles</t>
@@ -351,6 +345,36 @@
   </si>
   <si>
     <t>Percentage of target population using the OO app</t>
+  </si>
+  <si>
+    <t>Percentage of contacts detected by the OO app</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Time unit of simulation (if change, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>UPDATE G4 value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>seconds (DO NOT CHANGE THIS UNIT)</t>
   </si>
 </sst>
 </file>
@@ -506,7 +530,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -516,6 +539,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -737,8 +763,8 @@
   </sheetPr>
   <dimension ref="A1:AA1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -748,7 +774,7 @@
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" customWidth="1"/>
     <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -760,7 +786,7 @@
       <c r="C1" s="21"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -826,10 +852,10 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -860,21 +886,21 @@
       <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>0.5</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="6">
+        <v>76</v>
+      </c>
+      <c r="G4" s="31">
         <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -938,15 +964,15 @@
       <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -1099,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="3"/>
@@ -1162,14 +1188,14 @@
       <c r="B12" s="21"/>
       <c r="C12" s="20"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="28" t="s">
         <v>70</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
@@ -1203,14 +1229,14 @@
         <v>0.3</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="29" t="s">
-        <v>103</v>
+      <c r="E13" s="28" t="s">
+        <v>101</v>
       </c>
       <c r="F13" s="5">
         <v>100</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="3"/>
@@ -1244,14 +1270,15 @@
         <v>0.6</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="5" t="s">
         <v>102</v>
       </c>
       <c r="F14" s="5">
-        <f>G4*60/F19</f>
-        <v>1800</v>
-      </c>
-      <c r="G14" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1284,8 +1311,15 @@
         <v>0.4</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="F15" s="26"/>
-      <c r="H15" s="3"/>
+      <c r="E15" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="5">
+        <f>G4*60/F20</f>
+        <v>1800</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1317,12 +1351,6 @@
         <v>0.6</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1354,7 +1382,9 @@
         <v>0.1</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -1381,7 +1411,7 @@
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="20">
         <f>C5+C14+(1-C14+C14*C15)*C7</f>
@@ -1415,22 +1445,16 @@
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="20">
         <f>C23*(C13*(C8-C18)+C18)</f>
-        <v>0.2735104091888011</v>
+        <v>0.8205312275664034</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="7">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -1455,16 +1479,22 @@
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="20">
-        <f>C3*(100/F13)</f>
-        <v>7</v>
+        <f>C3*(100/F13)*(100/F14)</f>
+        <v>9.3333333333333321</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="H20" s="7"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1487,9 +1517,9 @@
       <c r="AA20" s="3"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1555,7 +1585,7 @@
       </c>
       <c r="C23" s="10">
         <f>F3/(F6*(C4+C13*(C8-C18)+C18))</f>
-        <v>0.11964584828906435</v>
+        <v>0.35893754486719309</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="7"/>
@@ -1590,8 +1620,8 @@
         <v>44</v>
       </c>
       <c r="C24" s="10">
-        <f>(C20*F10)/(F12*F9*C19*F14)</f>
-        <v>2.8436862058909313E-3</v>
+        <f>(C20*F10)/(F12*F9*C19*F15)</f>
+        <v>1.2638605359515244E-3</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="7"/>
@@ -1625,7 +1655,7 @@
       </c>
       <c r="C25" s="10">
         <f>C9*C24</f>
-        <v>2.8436862058909313E-3</v>
+        <v>1.2638605359515244E-3</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="7"/>
@@ -1659,7 +1689,7 @@
       </c>
       <c r="C26" s="10">
         <f>C10*C24</f>
-        <v>2.8436862058909313E-3</v>
+        <v>1.2638605359515244E-3</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="7"/>
@@ -1693,7 +1723,7 @@
       </c>
       <c r="C27" s="10">
         <f>C11*C24</f>
-        <v>2.8436862058909313E-3</v>
+        <v>1.2638605359515244E-3</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="7"/>
@@ -1727,7 +1757,7 @@
       </c>
       <c r="C28" s="10">
         <f>C4*C23</f>
-        <v>5.9822924144532177E-2</v>
+        <v>0.17946877243359655</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="7"/>
@@ -1761,13 +1791,13 @@
       </c>
       <c r="C29" s="10">
         <f>C7*C23</f>
-        <v>0.23929169657812871</v>
+        <v>0.71787508973438618</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1795,15 +1825,13 @@
       </c>
       <c r="C30" s="10">
         <f>$C5*$C23</f>
-        <v>1.1964584828906437E-2</v>
+        <v>3.5893754486719311E-2</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1831,15 +1859,13 @@
       </c>
       <c r="C31" s="10">
         <f>C6*C23</f>
-        <v>1.7946877243359652E-3</v>
+        <v>5.3840631730078959E-3</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" s="12">
-        <v>0.3</v>
-      </c>
+      <c r="E31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="3"/>
@@ -1869,15 +1895,14 @@
       </c>
       <c r="C32" s="10">
         <f>$C8*$C23</f>
-        <v>0.35893754486719309</v>
+        <v>1.0768126346015792</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F32" s="12">
-        <f>$F31/($F3*$F14*60/$F19)</f>
-        <v>5.555555555555555E-6</v>
+        <v>0.3</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
@@ -1912,10 +1937,11 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F33" s="12">
-        <v>2</v>
+        <f>$F32/($F3*$F15*60/$F20)</f>
+        <v>2.7777777777777775E-6</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
@@ -1942,7 +1968,7 @@
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D34" s="3"/>
       <c r="E34" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F34" s="12">
         <v>2</v>
@@ -1975,10 +2001,10 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F35" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -2008,10 +2034,10 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>27</v>
+        <v>41</v>
+      </c>
+      <c r="F36" s="12">
+        <v>1</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
@@ -2037,10 +2063,14 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="E37" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2064,7 +2094,7 @@
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13"/>
       <c r="B38" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="3"/>
@@ -2099,7 +2129,7 @@
       </c>
       <c r="C39" s="15">
         <f>C3/C19</f>
-        <v>25.593175853018376</v>
+        <v>8.5310586176727909</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -2133,7 +2163,7 @@
       </c>
       <c r="C40" s="13">
         <f>1/C19</f>
-        <v>3.6561679790026256</v>
+        <v>1.2187226596675416</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -2167,7 +2197,7 @@
       </c>
       <c r="C41" s="13">
         <f>1/C28</f>
-        <v>16.716000000000001</v>
+        <v>5.5720000000000001</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -30591,7 +30621,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -30649,7 +30679,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>60</v>
       </c>
     </row>
@@ -30807,7 +30837,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -30863,7 +30893,7 @@
       <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28"/>
+      <c r="A28" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31016,7 +31046,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>54</v>
       </c>
     </row>
@@ -31074,17 +31104,17 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="27" t="s">
         <v>66</v>
       </c>
     </row>
@@ -31113,7 +31143,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31243,8 +31273,8 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
-        <v>80</v>
+      <c r="B19" s="26" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
@@ -31276,7 +31306,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
@@ -31292,7 +31322,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
@@ -31301,17 +31331,17 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="27" t="s">
         <v>66</v>
       </c>
     </row>
@@ -31340,7 +31370,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31470,7 +31500,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>54</v>
       </c>
     </row>
@@ -31503,7 +31533,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
@@ -31519,7 +31549,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
@@ -31528,15 +31558,15 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28" t="s">
-        <v>86</v>
+      <c r="A28" s="27" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="28"/>
+      <c r="A29" s="27"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="28"/>
+      <c r="A30" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31559,7 +31589,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31689,8 +31719,8 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
-        <v>80</v>
+      <c r="B19" s="26" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
@@ -31722,7 +31752,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
@@ -31738,20 +31768,20 @@
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28"/>
+      <c r="A28" s="27"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="28"/>
+      <c r="A29" s="27"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="28"/>
+      <c r="A30" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31774,7 +31804,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -31904,7 +31934,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>54</v>
       </c>
     </row>
@@ -31937,7 +31967,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
@@ -31953,7 +31983,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
@@ -31962,18 +31992,18 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" s="27" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="28" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -31997,7 +32027,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19"/>
@@ -32127,7 +32157,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -32183,13 +32213,13 @@
       <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="28"/>
+      <c r="A28" s="27"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="28"/>
+      <c r="A29" s="27"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="28"/>
+      <c r="A30" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
use ceff as an auxiliary parameter
</commit_message>
<xml_diff>
--- a/par-calculator.xlsx
+++ b/par-calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/code/operation-outbreak/oo-parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9FBF23-E0CE-7C45-A415-8EB30BDB45A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8FC1A84-F2F3-0447-B426-42E32074D1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="40940" windowHeight="22540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EPI Calculation Formulas" sheetId="1" r:id="rId1"/>
@@ -335,9 +335,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>HELPER VALUE R0 scaled (do not overwrite)</t>
-  </si>
-  <si>
     <t>Number of consecutive infections during simulation</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>seconds (DO NOT CHANGE THIS UNIT)</t>
+  </si>
+  <si>
+    <t>HELPER VALUE ceff, effective contact rate (do not overwrite)</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -538,7 +538,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -764,7 +763,7 @@
   <dimension ref="A1:AA1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -891,12 +890,12 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="30">
         <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -969,7 +968,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
@@ -1230,7 +1229,7 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="5">
         <v>100</v>
@@ -1271,7 +1270,7 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" s="5">
         <v>75</v>
@@ -1312,7 +1311,7 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="5">
         <f>G4*60/F20</f>
@@ -1479,11 +1478,11 @@
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="21" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C20" s="20">
-        <f>C3*(100/F13)*(100/F14)</f>
-        <v>9.3333333333333321</v>
+        <f>(F9/F10)*(F13/100)*(F14/100)</f>
+        <v>3.75</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="7" t="s">
@@ -1493,7 +1492,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="3"/>
@@ -1517,9 +1516,9 @@
       <c r="AA20" s="3"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1620,8 +1619,8 @@
         <v>44</v>
       </c>
       <c r="C24" s="10">
-        <f>(C20*F10)/(F12*F9*C19*F15)</f>
-        <v>1.2638605359515244E-3</v>
+        <f>(C3)/(F12*C20*C19*F15)</f>
+        <v>1.2638605359515246E-3</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="7"/>
@@ -1655,7 +1654,7 @@
       </c>
       <c r="C25" s="10">
         <f>C9*C24</f>
-        <v>1.2638605359515244E-3</v>
+        <v>1.2638605359515246E-3</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="7"/>
@@ -1689,7 +1688,7 @@
       </c>
       <c r="C26" s="10">
         <f>C10*C24</f>
-        <v>1.2638605359515244E-3</v>
+        <v>1.2638605359515246E-3</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="7"/>
@@ -1723,7 +1722,7 @@
       </c>
       <c r="C27" s="10">
         <f>C11*C24</f>
-        <v>1.2638605359515244E-3</v>
+        <v>1.2638605359515246E-3</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="7"/>

</xml_diff>